<commit_message>
Update PM15 Tidsregistrering for Laila.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM15 Tidsregistrering for Laila.xlsx
+++ b/08 Project Management/Tidsregistrering/PM15 Tidsregistrering for Laila.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laila\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898B1C26-95F2-4CB3-805C-809F71068D0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33E793A-2607-4B03-9D13-59B643B751A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -800,7 +800,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1109,42 +1109,68 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E12" s="16">
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>1.041666666666663E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.74652777777777779</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="A13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="15">
+        <v>43893</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="F13" s="20"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.24999999999999994</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0277777777777777</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C14" s="15"/>
+      <c r="A14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="15">
+        <v>43893</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E14" s="17">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F14" s="20"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1156,7 +1182,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1168,7 +1194,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1180,7 +1206,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1192,7 +1218,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1204,7 +1230,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1216,7 +1242,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1228,7 +1254,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1240,7 +1266,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1252,7 +1278,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1264,7 +1290,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1275,7 +1301,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1286,7 +1312,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1297,7 +1323,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1308,7 +1334,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1319,7 +1345,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1330,7 +1356,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1341,7 +1367,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1352,7 +1378,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.74652777777777779</v>
+        <v>1.0902777777777777</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>